<commit_message>
DiagonalBorder and DiagonalBorderColor added to comparision. Reference file fixed
</commit_message>
<xml_diff>
--- a/ClosedXML_Tests/Resource/Examples/Styles/StyleBorder.xlsx
+++ b/ClosedXML_Tests/Resource/Examples/Styles/StyleBorder.xlsx
@@ -61,7 +61,7 @@
       <x:patternFill patternType="gray125"/>
     </x:fill>
   </x:fills>
-  <x:borders count="11">
+  <x:borders count="8">
     <x:border diagonalUp="0" diagonalDown="0">
       <x:left style="none">
         <x:color rgb="FF000000"/>
@@ -198,59 +198,8 @@
         <x:color rgb="FFFF0000"/>
       </x:diagonal>
     </x:border>
-    <x:border diagonalUp="1" diagonalDown="0">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="thin">
-        <x:color rgb="FFFF0000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="0" diagonalDown="1">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="thin">
-        <x:color rgb="FFFF0000"/>
-      </x:diagonal>
-    </x:border>
-    <x:border diagonalUp="1" diagonalDown="1">
-      <x:left style="none">
-        <x:color rgb="FF000000"/>
-      </x:left>
-      <x:right style="none">
-        <x:color rgb="FF000000"/>
-      </x:right>
-      <x:top style="none">
-        <x:color rgb="FF000000"/>
-      </x:top>
-      <x:bottom style="none">
-        <x:color rgb="FF000000"/>
-      </x:bottom>
-      <x:diagonal style="thin">
-        <x:color rgb="FFFF0000"/>
-      </x:diagonal>
-    </x:border>
   </x:borders>
-  <x:cellStyleXfs count="11">
+  <x:cellStyleXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -275,17 +224,8 @@
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="8" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="9" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
   </x:cellStyleXfs>
-  <x:cellXfs count="11">
+  <x:cellXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
@@ -315,18 +255,6 @@
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
@@ -652,17 +580,17 @@
       </x:c>
     </x:row>
     <x:row r="6" spans="1:2">
-      <x:c r="B6" s="8" t="s">
+      <x:c r="B6" s="5" t="s">
         <x:v>4</x:v>
       </x:c>
     </x:row>
     <x:row r="7" spans="1:2">
-      <x:c r="B7" s="9" t="s">
+      <x:c r="B7" s="6" t="s">
         <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="8" spans="1:2">
-      <x:c r="B8" s="10" t="s">
+      <x:c r="B8" s="7" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>

</xml_diff>